<commit_message>
Updated Founder David Le
</commit_message>
<xml_diff>
--- a/res/david_le.xlsx
+++ b/res/david_le.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aruksh/Google Drive/Personal/Projects and Practices/Lineage_Tree/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA484410-2C31-114D-B6C8-254D21960F81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54A1B7D-5958-A44D-9C53-26F8E8CDC13A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10000" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,9 +566,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -924,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +934,7 @@
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,7 +945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>4</v>
       </c>
@@ -957,7 +956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>30</v>
       </c>
@@ -968,7 +967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>48</v>
       </c>
@@ -979,7 +978,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>56</v>
       </c>
@@ -990,7 +989,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>65</v>
       </c>
@@ -1001,7 +1000,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>75</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>81</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>97</v>
       </c>
@@ -1033,9 +1032,8 @@
       <c r="C9">
         <v>81</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>116</v>
       </c>
@@ -1046,7 +1044,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>136</v>
       </c>
@@ -1057,7 +1055,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>152</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>158</v>
       </c>
@@ -1079,7 +1077,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>169</v>
       </c>
@@ -1090,7 +1088,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>176</v>
       </c>
@@ -1101,7 +1099,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>120</v>
       </c>

</xml_diff>